<commit_message>
updates to hydro progress.
</commit_message>
<xml_diff>
--- a/doc/project_management/tracking_hydrowork.xlsx
+++ b/doc/project_management/tracking_hydrowork.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnel\Documents\Project\G2G_supplyshed\doc\project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D62754A-665B-4CC6-87EC-5D9CAE74C449}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92DB95F-B52A-43A3-A892-FDCAB72299F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8220" yWindow="852" windowWidth="17280" windowHeight="8976" xr2:uid="{C39EBF64-7E6C-46AF-9D79-6A233BCEB030}"/>
+    <workbookView xWindow="8220" yWindow="855" windowWidth="17280" windowHeight="8970" xr2:uid="{C39EBF64-7E6C-46AF-9D79-6A233BCEB030}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -506,18 +506,18 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>70801030408</v>
       </c>
@@ -557,7 +557,7 @@
         <v>100.00009791825784</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>70802060502</v>
       </c>
@@ -580,7 +580,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>70801030303</v>
       </c>
@@ -603,7 +603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>70801030409</v>
       </c>
@@ -620,7 +620,7 @@
         <v>88.246393602762438</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>70802060601</v>
       </c>
@@ -643,7 +643,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>70801030407</v>
       </c>
@@ -666,7 +666,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>70802060501</v>
       </c>
@@ -683,7 +683,7 @@
         <v>71.74410906751379</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>70801030302</v>
       </c>
@@ -700,13 +700,13 @@
         <v>56.256013658330005</v>
       </c>
       <c r="F9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>70801030301</v>
       </c>
@@ -729,7 +729,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>70802060603</v>
       </c>
@@ -746,7 +746,7 @@
         <v>39.823590255950784</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>70801030406</v>
       </c>
@@ -763,7 +763,7 @@
         <v>25.918384738050172</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>70802060503</v>
       </c>
@@ -780,7 +780,7 @@
         <v>17.939764120915076</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>70801030603</v>
       </c>
@@ -797,7 +797,7 @@
         <v>8.3674223176751372</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>70801010602</v>
       </c>
@@ -814,7 +814,7 @@
         <v>2.6567894656481341</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>70802060602</v>
       </c>
@@ -831,7 +831,7 @@
         <v>2.3643701593641997</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>70801030404</v>
       </c>
@@ -848,7 +848,7 @@
         <v>1.93220273423515</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>70801030405</v>
       </c>

</xml_diff>

<commit_message>
update to hydro progress.
</commit_message>
<xml_diff>
--- a/doc/project_management/tracking_hydrowork.xlsx
+++ b/doc/project_management/tracking_hydrowork.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnel\Documents\Project\G2G_supplyshed\doc\project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92DB95F-B52A-43A3-A892-FDCAB72299F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FA526D-4AA4-435F-98AB-EFE7EAA6A3A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8220" yWindow="855" windowWidth="17280" windowHeight="8970" xr2:uid="{C39EBF64-7E6C-46AF-9D79-6A233BCEB030}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>HUC12</t>
   </si>
@@ -503,7 +503,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,6 +556,12 @@
       <c r="E2" s="4">
         <v>100.00009791825784</v>
       </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -574,7 +580,7 @@
         <v>98.990728560918612</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
updates and additions to project documents.
</commit_message>
<xml_diff>
--- a/doc/project_management/tracking_hydrowork.xlsx
+++ b/doc/project_management/tracking_hydrowork.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnel\Documents\Project\G2G_supplyshed\doc\project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FA526D-4AA4-435F-98AB-EFE7EAA6A3A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B54D69-7685-497B-BAA6-66C1400D9CA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8220" yWindow="855" windowWidth="17280" windowHeight="8970" xr2:uid="{C39EBF64-7E6C-46AF-9D79-6A233BCEB030}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>HUC12</t>
   </si>
@@ -503,7 +503,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +557,7 @@
         <v>100.00009791825784</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
         <v>27</v>
@@ -624,6 +624,12 @@
       </c>
       <c r="E5" s="4">
         <v>88.246393602762438</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>